<commit_message>
chore: update Excel kuliner
</commit_message>
<xml_diff>
--- a/excel/wedago_kuliner_master_final.xlsx
+++ b/excel/wedago_kuliner_master_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEDAGO\INPUTAN\HTML\INPUT KULINER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61D309D-71D7-43E7-90E1-7CDD9137FC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60167F07-7E1E-4F00-A458-BBD6FA083A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Dictionary" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Data!$A$1:$P$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Data!$A$1:$P$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="390">
   <si>
     <t>judul</t>
   </si>
@@ -460,108 +460,6 @@
   </si>
   <si>
     <t>https://jgjk.mobi/p/68be02efa38d5</t>
-  </si>
-  <si>
-    <t>Menu Tradisional</t>
-  </si>
-  <si>
-    <t>Berbagai Menu Khas Halmahera Tengah</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Menu-Tradisional-0-21268bd14f877673.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd14f877673</t>
-  </si>
-  <si>
-    <t>Seafod</t>
-  </si>
-  <si>
-    <t>Serba Hidangan Laut</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Seafod-0-73968bd0f33c527a.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0f33c527a</t>
-  </si>
-  <si>
-    <t>Serba Kopi</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Kopi-0-91568bd0eebdb8db.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0eebdb8db</t>
-  </si>
-  <si>
-    <t>Serba Sarapan</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Sarapan-0-40968bd0c67b99c9.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0c67b99c9</t>
-  </si>
-  <si>
-    <t>Roti Dan Kue</t>
-  </si>
-  <si>
-    <t>Serba Roti</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Roti-0-53968bd0c0e104e1.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0c0e104e1</t>
-  </si>
-  <si>
-    <t>Bakso Dan Mie</t>
-  </si>
-  <si>
-    <t>Serba Bakso dan Mie</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Bakso-Dan-Mie-0-90468bd0baeae98e.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0baeae98e</t>
-  </si>
-  <si>
-    <t>Serba Cemilan</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Cemilan-0-72868bd0b5a13f91.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0b5a13f91</t>
-  </si>
-  <si>
-    <t>Serba Minuman</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Minuman-0-37568bd0b134d2e9.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0b134d2e9</t>
-  </si>
-  <si>
-    <t>Serba Ayam</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Ayam-0-87968bd0a0611720.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0a0611720</t>
-  </si>
-  <si>
-    <t>Serba Nasi</t>
-  </si>
-  <si>
-    <t>https://umkmdigital.app/api/listimage/v/Nasi-0-48568bd0999cc25b.jpg</t>
-  </si>
-  <si>
-    <t>https://jgjk.mobi/p/68bd0999cc25b</t>
   </si>
   <si>
     <t>Es Capci</t>
@@ -1940,10 +1838,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K5" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="O60" sqref="O60"/>
+    <sheetView tabSelected="1" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2381,7 +2279,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -2389,16 +2287,22 @@
         <v>142</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E12" t="s">
         <v>143</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="H12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" t="s">
+        <v>125</v>
       </c>
       <c r="J12" t="s">
         <v>85</v>
@@ -2409,25 +2313,37 @@
       <c r="L12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="M12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C13">
+        <v>25000</v>
+      </c>
+      <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="G13" t="s">
-        <v>148</v>
+        <v>150</v>
+      </c>
+      <c r="H13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" t="s">
+        <v>125</v>
       </c>
       <c r="J13" t="s">
         <v>85</v>
@@ -2438,25 +2354,37 @@
       <c r="L13" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="M13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C14">
+        <v>30000</v>
+      </c>
+      <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="G14" t="s">
-        <v>151</v>
+        <v>155</v>
+      </c>
+      <c r="H14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" t="s">
+        <v>125</v>
       </c>
       <c r="J14" t="s">
         <v>85</v>
@@ -2468,27 +2396,36 @@
         <v>87</v>
       </c>
       <c r="M14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C15">
+        <v>30000</v>
+      </c>
+      <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="G15" t="s">
-        <v>154</v>
+        <v>160</v>
+      </c>
+      <c r="H15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" t="s">
+        <v>125</v>
       </c>
       <c r="J15" t="s">
         <v>85</v>
@@ -2499,118 +2436,154 @@
       <c r="L15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="M15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C16">
+        <v>20000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" t="s">
+        <v>85</v>
+      </c>
+      <c r="K16" t="s">
+        <v>86</v>
+      </c>
+      <c r="L16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17">
+        <v>20000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" t="s">
+        <v>169</v>
+      </c>
+      <c r="G17" t="s">
+        <v>170</v>
+      </c>
+      <c r="H17" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18">
+        <v>30000</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
-        <v>157</v>
-      </c>
-      <c r="F16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" t="s">
-        <v>158</v>
-      </c>
-      <c r="J16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K16" t="s">
-        <v>86</v>
-      </c>
-      <c r="L16" t="s">
-        <v>87</v>
-      </c>
-      <c r="M16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>159</v>
-      </c>
-      <c r="B17" t="s">
-        <v>160</v>
-      </c>
-      <c r="C17">
+      <c r="E18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" t="s">
+        <v>86</v>
+      </c>
+      <c r="L18" t="s">
+        <v>87</v>
+      </c>
+      <c r="M18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19">
+        <v>20000</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
-        <v>161</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" t="s">
-        <v>162</v>
-      </c>
-      <c r="J17" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" t="s">
-        <v>87</v>
-      </c>
-      <c r="M17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" t="s">
-        <v>163</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>164</v>
-      </c>
-      <c r="F18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" t="s">
-        <v>165</v>
-      </c>
-      <c r="J18" t="s">
-        <v>85</v>
-      </c>
-      <c r="K18" t="s">
-        <v>86</v>
-      </c>
-      <c r="L18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>166</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
       <c r="E19" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
       <c r="G19" t="s">
-        <v>168</v>
+        <v>180</v>
+      </c>
+      <c r="H19" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" t="s">
+        <v>125</v>
       </c>
       <c r="J19" t="s">
         <v>85</v>
@@ -2621,25 +2594,34 @@
       <c r="L19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="M19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>25000</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
       <c r="G20" t="s">
-        <v>171</v>
+        <v>185</v>
+      </c>
+      <c r="H20" t="s">
+        <v>186</v>
       </c>
       <c r="J20" t="s">
         <v>85</v>
@@ -2650,28 +2632,31 @@
       <c r="L20" t="s">
         <v>87</v>
       </c>
-      <c r="M20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>25000</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="G21" t="s">
-        <v>174</v>
+        <v>190</v>
+      </c>
+      <c r="H21" t="s">
+        <v>186</v>
       </c>
       <c r="J21" t="s">
         <v>85</v>
@@ -2681,35 +2666,32 @@
       </c>
       <c r="L21" t="s">
         <v>87</v>
-      </c>
-      <c r="M21" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C22">
-        <v>10000</v>
+        <v>30000</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F22" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="G22" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="H22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I22" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="J22" t="s">
         <v>85</v>
@@ -2721,36 +2703,33 @@
         <v>87</v>
       </c>
       <c r="M22" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C23">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="F23" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="G23" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="H23" t="s">
-        <v>124</v>
-      </c>
-      <c r="I23" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="J23" t="s">
         <v>85</v>
@@ -2760,38 +2739,32 @@
       </c>
       <c r="L23" t="s">
         <v>87</v>
-      </c>
-      <c r="M23" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C24">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="F24" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="G24" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="H24" t="s">
-        <v>124</v>
-      </c>
-      <c r="I24" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="J24" t="s">
         <v>85</v>
@@ -2803,36 +2776,33 @@
         <v>87</v>
       </c>
       <c r="M24" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C25">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="G25" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="H25" t="s">
-        <v>124</v>
-      </c>
-      <c r="I25" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="J25" t="s">
         <v>85</v>
@@ -2844,33 +2814,33 @@
         <v>87</v>
       </c>
       <c r="M25" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C26">
-        <v>20000</v>
+        <v>25000</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="F26" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="G26" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="H26" t="s">
-        <v>124</v>
-      </c>
-      <c r="I26" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="J26" t="s">
         <v>85</v>
@@ -2880,35 +2850,32 @@
       </c>
       <c r="L26" t="s">
         <v>87</v>
-      </c>
-      <c r="M26" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="B27" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="C27">
-        <v>20000</v>
+        <v>25000</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="F27" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="G27" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="H27" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="J27" t="s">
         <v>85</v>
@@ -2918,38 +2885,32 @@
       </c>
       <c r="L27" t="s">
         <v>87</v>
-      </c>
-      <c r="M27" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="B28" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="C28">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="F28" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="G28" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="H28" t="s">
-        <v>124</v>
-      </c>
-      <c r="I28" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="J28" t="s">
         <v>85</v>
@@ -2961,36 +2922,33 @@
         <v>87</v>
       </c>
       <c r="M28" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C29">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="F29" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="G29" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="H29" t="s">
-        <v>124</v>
-      </c>
-      <c r="I29" t="s">
-        <v>125</v>
+        <v>225</v>
       </c>
       <c r="J29" t="s">
         <v>85</v>
@@ -3000,35 +2958,32 @@
       </c>
       <c r="L29" t="s">
         <v>87</v>
-      </c>
-      <c r="M29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
       <c r="C30">
-        <v>25000</v>
+        <v>15000</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="F30" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="G30" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="H30" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="J30" t="s">
         <v>85</v>
@@ -3042,28 +2997,28 @@
     </row>
     <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
       <c r="C31">
-        <v>25000</v>
+        <v>15000</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F31" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="G31" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H31" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="J31" t="s">
         <v>85</v>
@@ -3077,28 +3032,28 @@
     </row>
     <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="C32">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="F32" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G32" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="H32" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="J32" t="s">
         <v>85</v>
@@ -3108,35 +3063,32 @@
       </c>
       <c r="L32" t="s">
         <v>87</v>
-      </c>
-      <c r="M32" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B33" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C33">
-        <v>20000</v>
+        <v>35000</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E33" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="F33" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="G33" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="H33" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="J33" t="s">
         <v>85</v>
@@ -3150,28 +3102,28 @@
     </row>
     <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="B34" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="C34">
-        <v>20000</v>
+        <v>2500</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="F34" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="G34" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="H34" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="J34" t="s">
         <v>85</v>
@@ -3183,33 +3135,33 @@
         <v>87</v>
       </c>
       <c r="M34" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="C35">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="E35" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="F35" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="G35" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="H35" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="J35" t="s">
         <v>85</v>
@@ -3221,33 +3173,33 @@
         <v>87</v>
       </c>
       <c r="M35" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B36" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="C36">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="F36" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="G36" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="H36" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="J36" t="s">
         <v>85</v>
@@ -3259,30 +3211,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>114</v>
       </c>
       <c r="C37">
-        <v>25000</v>
-      </c>
-      <c r="D37">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="F37" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="G37" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="H37" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="J37" t="s">
         <v>85</v>
@@ -3296,66 +3245,63 @@
     </row>
     <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="C38">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D38">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>264</v>
+      </c>
+      <c r="F38" t="s">
+        <v>265</v>
+      </c>
+      <c r="G38" t="s">
+        <v>266</v>
+      </c>
+      <c r="H38" t="s">
+        <v>267</v>
+      </c>
+      <c r="J38" t="s">
+        <v>85</v>
+      </c>
+      <c r="K38" t="s">
+        <v>86</v>
+      </c>
+      <c r="L38" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>268</v>
+      </c>
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39">
         <v>0</v>
       </c>
-      <c r="E38" t="s">
-        <v>251</v>
-      </c>
-      <c r="F38" t="s">
-        <v>252</v>
-      </c>
-      <c r="G38" t="s">
-        <v>253</v>
-      </c>
-      <c r="H38" t="s">
-        <v>220</v>
-      </c>
-      <c r="J38" t="s">
-        <v>85</v>
-      </c>
-      <c r="K38" t="s">
-        <v>86</v>
-      </c>
-      <c r="L38" t="s">
-        <v>87</v>
-      </c>
-      <c r="M38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>254</v>
-      </c>
-      <c r="B39" t="s">
-        <v>255</v>
-      </c>
-      <c r="C39">
-        <v>10000</v>
-      </c>
-      <c r="D39">
-        <v>9</v>
-      </c>
       <c r="E39" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="F39" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="G39" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="H39" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="J39" t="s">
         <v>85</v>
@@ -3366,31 +3312,31 @@
       <c r="L39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+      <c r="M39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>114</v>
       </c>
       <c r="C40">
-        <v>15000</v>
-      </c>
-      <c r="D40">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F40" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="G40" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="H40" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="J40" t="s">
         <v>85</v>
@@ -3402,30 +3348,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>114</v>
       </c>
       <c r="C41">
-        <v>15000</v>
-      </c>
-      <c r="D41">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="F41" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="G41" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="H41" t="s">
-        <v>264</v>
+        <v>118</v>
       </c>
       <c r="J41" t="s">
         <v>85</v>
@@ -3436,31 +3379,31 @@
       <c r="L41" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+      <c r="M41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="C42">
-        <v>25000</v>
-      </c>
-      <c r="D42">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
         <v>269</v>
       </c>
       <c r="F42" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="G42" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="H42" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="J42" t="s">
         <v>85</v>
@@ -3470,32 +3413,38 @@
       </c>
       <c r="L42" t="s">
         <v>87</v>
+      </c>
+      <c r="M42" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="B43" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="C43">
-        <v>35000</v>
+        <v>30000</v>
       </c>
       <c r="D43">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="F43" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="G43" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="H43" t="s">
-        <v>272</v>
+        <v>124</v>
+      </c>
+      <c r="I43" t="s">
+        <v>125</v>
       </c>
       <c r="J43" t="s">
         <v>85</v>
@@ -3505,32 +3454,38 @@
       </c>
       <c r="L43" t="s">
         <v>87</v>
+      </c>
+      <c r="M43" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="B44" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="C44">
-        <v>2500</v>
+        <v>20000</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="F44" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="G44" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="H44" t="s">
-        <v>282</v>
+        <v>124</v>
+      </c>
+      <c r="I44" t="s">
+        <v>125</v>
       </c>
       <c r="J44" t="s">
         <v>85</v>
@@ -3542,33 +3497,36 @@
         <v>87</v>
       </c>
       <c r="M44" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="B45" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="C45">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="D45">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="F45" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="G45" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="H45" t="s">
-        <v>282</v>
+        <v>124</v>
+      </c>
+      <c r="I45" t="s">
+        <v>125</v>
       </c>
       <c r="J45" t="s">
         <v>85</v>
@@ -3578,102 +3536,105 @@
       </c>
       <c r="L45" t="s">
         <v>87</v>
-      </c>
-      <c r="M45" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B46" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="C46">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D46">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>302</v>
+      </c>
+      <c r="F46" t="s">
+        <v>303</v>
+      </c>
+      <c r="G46" t="s">
+        <v>304</v>
+      </c>
+      <c r="H46" t="s">
+        <v>186</v>
+      </c>
+      <c r="J46" t="s">
+        <v>85</v>
+      </c>
+      <c r="K46" t="s">
+        <v>86</v>
+      </c>
+      <c r="L46" t="s">
+        <v>87</v>
+      </c>
+      <c r="M46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>305</v>
+      </c>
+      <c r="B47" t="s">
+        <v>301</v>
+      </c>
+      <c r="C47">
+        <v>20000</v>
+      </c>
+      <c r="D47">
         <v>20</v>
       </c>
-      <c r="E46" t="s">
-        <v>289</v>
-      </c>
-      <c r="F46" t="s">
-        <v>290</v>
-      </c>
-      <c r="G46" t="s">
-        <v>291</v>
-      </c>
-      <c r="H46" t="s">
-        <v>272</v>
-      </c>
-      <c r="J46" t="s">
-        <v>85</v>
-      </c>
-      <c r="K46" t="s">
-        <v>86</v>
-      </c>
-      <c r="L46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>292</v>
-      </c>
-      <c r="B47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47">
+      <c r="E47" t="s">
+        <v>306</v>
+      </c>
+      <c r="F47" t="s">
+        <v>307</v>
+      </c>
+      <c r="G47" t="s">
+        <v>308</v>
+      </c>
+      <c r="H47" t="s">
+        <v>186</v>
+      </c>
+      <c r="J47" t="s">
+        <v>85</v>
+      </c>
+      <c r="K47" t="s">
+        <v>86</v>
+      </c>
+      <c r="L47" t="s">
+        <v>87</v>
+      </c>
+      <c r="M47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>309</v>
+      </c>
+      <c r="B48" t="s">
+        <v>310</v>
+      </c>
+      <c r="C48">
         <v>0</v>
       </c>
-      <c r="E47" t="s">
-        <v>293</v>
-      </c>
-      <c r="F47" t="s">
-        <v>294</v>
-      </c>
-      <c r="G47" t="s">
-        <v>295</v>
-      </c>
-      <c r="H47" t="s">
-        <v>296</v>
-      </c>
-      <c r="J47" t="s">
-        <v>85</v>
-      </c>
-      <c r="K47" t="s">
-        <v>86</v>
-      </c>
-      <c r="L47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>297</v>
-      </c>
-      <c r="B48" t="s">
-        <v>278</v>
-      </c>
-      <c r="C48">
-        <v>30000</v>
-      </c>
-      <c r="D48">
-        <v>20</v>
-      </c>
       <c r="E48" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="F48" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="G48" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="H48" t="s">
-        <v>301</v>
+        <v>105</v>
       </c>
       <c r="J48" t="s">
         <v>85</v>
@@ -3685,30 +3646,33 @@
         <v>87</v>
       </c>
       <c r="M48" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>315</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="F49" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="G49" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="H49" t="s">
-        <v>306</v>
+        <v>277</v>
+      </c>
+      <c r="I49" t="s">
+        <v>125</v>
       </c>
       <c r="J49" t="s">
         <v>85</v>
@@ -3720,30 +3684,30 @@
         <v>87</v>
       </c>
       <c r="M49" t="s">
-        <v>33</v>
+        <v>388</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>320</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>308</v>
+        <v>269</v>
       </c>
       <c r="F50" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="G50" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="H50" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="J50" t="s">
         <v>85</v>
@@ -3753,11 +3717,14 @@
       </c>
       <c r="L50" t="s">
         <v>87</v>
+      </c>
+      <c r="M50" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="B51" t="s">
         <v>114</v>
@@ -3766,13 +3733,13 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="F51" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="G51" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="H51" t="s">
         <v>118</v>
@@ -3787,385 +3754,11 @@
         <v>87</v>
       </c>
       <c r="M51" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>316</v>
-      </c>
-      <c r="B52" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="E52" t="s">
-        <v>303</v>
-      </c>
-      <c r="F52" t="s">
-        <v>317</v>
-      </c>
-      <c r="G52" t="s">
-        <v>318</v>
-      </c>
-      <c r="H52" t="s">
-        <v>311</v>
-      </c>
-      <c r="J52" t="s">
-        <v>85</v>
-      </c>
-      <c r="K52" t="s">
-        <v>86</v>
-      </c>
-      <c r="L52" t="s">
-        <v>87</v>
-      </c>
-      <c r="M52" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>319</v>
-      </c>
-      <c r="B53" t="s">
-        <v>320</v>
-      </c>
-      <c r="C53">
-        <v>30000</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53" t="s">
-        <v>321</v>
-      </c>
-      <c r="F53" t="s">
-        <v>322</v>
-      </c>
-      <c r="G53" t="s">
-        <v>323</v>
-      </c>
-      <c r="H53" t="s">
-        <v>124</v>
-      </c>
-      <c r="I53" t="s">
-        <v>125</v>
-      </c>
-      <c r="J53" t="s">
-        <v>85</v>
-      </c>
-      <c r="K53" t="s">
-        <v>86</v>
-      </c>
-      <c r="L53" t="s">
-        <v>87</v>
-      </c>
-      <c r="M53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>324</v>
-      </c>
-      <c r="B54" t="s">
-        <v>325</v>
-      </c>
-      <c r="C54">
-        <v>20000</v>
-      </c>
-      <c r="D54">
-        <v>20</v>
-      </c>
-      <c r="E54" t="s">
-        <v>326</v>
-      </c>
-      <c r="F54" t="s">
-        <v>327</v>
-      </c>
-      <c r="G54" t="s">
-        <v>328</v>
-      </c>
-      <c r="H54" t="s">
-        <v>124</v>
-      </c>
-      <c r="I54" t="s">
-        <v>125</v>
-      </c>
-      <c r="J54" t="s">
-        <v>85</v>
-      </c>
-      <c r="K54" t="s">
-        <v>86</v>
-      </c>
-      <c r="L54" t="s">
-        <v>87</v>
-      </c>
-      <c r="M54" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>329</v>
-      </c>
-      <c r="B55" t="s">
-        <v>330</v>
-      </c>
-      <c r="C55">
-        <v>25000</v>
-      </c>
-      <c r="D55">
-        <v>20</v>
-      </c>
-      <c r="E55" t="s">
-        <v>331</v>
-      </c>
-      <c r="F55" t="s">
-        <v>332</v>
-      </c>
-      <c r="G55" t="s">
-        <v>333</v>
-      </c>
-      <c r="H55" t="s">
-        <v>124</v>
-      </c>
-      <c r="I55" t="s">
-        <v>125</v>
-      </c>
-      <c r="J55" t="s">
-        <v>85</v>
-      </c>
-      <c r="K55" t="s">
-        <v>86</v>
-      </c>
-      <c r="L55" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>334</v>
-      </c>
-      <c r="B56" t="s">
-        <v>335</v>
-      </c>
-      <c r="C56">
-        <v>20000</v>
-      </c>
-      <c r="D56">
-        <v>9</v>
-      </c>
-      <c r="E56" t="s">
-        <v>336</v>
-      </c>
-      <c r="F56" t="s">
-        <v>337</v>
-      </c>
-      <c r="G56" t="s">
-        <v>338</v>
-      </c>
-      <c r="H56" t="s">
-        <v>220</v>
-      </c>
-      <c r="J56" t="s">
-        <v>85</v>
-      </c>
-      <c r="K56" t="s">
-        <v>86</v>
-      </c>
-      <c r="L56" t="s">
-        <v>87</v>
-      </c>
-      <c r="M56" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>339</v>
-      </c>
-      <c r="B57" t="s">
-        <v>335</v>
-      </c>
-      <c r="C57">
-        <v>20000</v>
-      </c>
-      <c r="D57">
-        <v>20</v>
-      </c>
-      <c r="E57" t="s">
-        <v>340</v>
-      </c>
-      <c r="F57" t="s">
-        <v>341</v>
-      </c>
-      <c r="G57" t="s">
-        <v>342</v>
-      </c>
-      <c r="H57" t="s">
-        <v>220</v>
-      </c>
-      <c r="J57" t="s">
-        <v>85</v>
-      </c>
-      <c r="K57" t="s">
-        <v>86</v>
-      </c>
-      <c r="L57" t="s">
-        <v>87</v>
-      </c>
-      <c r="M57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>343</v>
-      </c>
-      <c r="B58" t="s">
-        <v>344</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="E58" t="s">
-        <v>345</v>
-      </c>
-      <c r="F58" t="s">
-        <v>346</v>
-      </c>
-      <c r="G58" t="s">
-        <v>347</v>
-      </c>
-      <c r="H58" t="s">
-        <v>105</v>
-      </c>
-      <c r="J58" t="s">
-        <v>85</v>
-      </c>
-      <c r="K58" t="s">
-        <v>86</v>
-      </c>
-      <c r="L58" t="s">
-        <v>87</v>
-      </c>
-      <c r="M58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>348</v>
-      </c>
-      <c r="B59" t="s">
-        <v>349</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="E59" t="s">
-        <v>350</v>
-      </c>
-      <c r="F59" t="s">
-        <v>351</v>
-      </c>
-      <c r="G59" t="s">
-        <v>352</v>
-      </c>
-      <c r="H59" t="s">
-        <v>311</v>
-      </c>
-      <c r="I59" t="s">
-        <v>125</v>
-      </c>
-      <c r="J59" t="s">
-        <v>85</v>
-      </c>
-      <c r="K59" t="s">
-        <v>86</v>
-      </c>
-      <c r="L59" t="s">
-        <v>87</v>
-      </c>
-      <c r="M59" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>353</v>
-      </c>
-      <c r="B60" t="s">
-        <v>354</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="E60" t="s">
-        <v>303</v>
-      </c>
-      <c r="F60" t="s">
-        <v>355</v>
-      </c>
-      <c r="G60" t="s">
-        <v>356</v>
-      </c>
-      <c r="H60" t="s">
-        <v>357</v>
-      </c>
-      <c r="J60" t="s">
-        <v>85</v>
-      </c>
-      <c r="K60" t="s">
-        <v>86</v>
-      </c>
-      <c r="L60" t="s">
-        <v>87</v>
-      </c>
-      <c r="M60" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>358</v>
-      </c>
-      <c r="B61" t="s">
-        <v>114</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="E61" t="s">
-        <v>359</v>
-      </c>
-      <c r="F61" t="s">
-        <v>360</v>
-      </c>
-      <c r="G61" t="s">
-        <v>361</v>
-      </c>
-      <c r="H61" t="s">
-        <v>118</v>
-      </c>
-      <c r="J61" t="s">
-        <v>85</v>
-      </c>
-      <c r="K61" t="s">
-        <v>86</v>
-      </c>
-      <c r="L61" t="s">
-        <v>87</v>
-      </c>
-      <c r="M61" t="s">
-        <v>423</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P61" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <autoFilter ref="A1:P51" xr:uid="{00000000-0001-0000-0200-000000000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="0"/>
@@ -4192,299 +3785,299 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>362</v>
+        <v>328</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>363</v>
+        <v>329</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>364</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>365</v>
+        <v>331</v>
       </c>
       <c r="B2" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C2" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C4" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>372</v>
+        <v>338</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C5" t="s">
-        <v>373</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
       <c r="B6" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C6" t="s">
-        <v>376</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>377</v>
+        <v>343</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C7" t="s">
-        <v>378</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="B8" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
       <c r="C8" t="s">
-        <v>381</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>382</v>
+        <v>348</v>
       </c>
       <c r="B9" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C9" t="s">
-        <v>383</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>384</v>
+        <v>350</v>
       </c>
       <c r="B10" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C10" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>386</v>
+        <v>352</v>
       </c>
       <c r="B11" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>388</v>
+        <v>354</v>
       </c>
       <c r="B12" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C12" t="s">
-        <v>389</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>390</v>
+        <v>356</v>
       </c>
       <c r="B13" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C13" t="s">
-        <v>391</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>392</v>
+        <v>358</v>
       </c>
       <c r="B14" t="s">
-        <v>393</v>
+        <v>359</v>
       </c>
       <c r="C14" t="s">
-        <v>394</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>395</v>
+        <v>361</v>
       </c>
       <c r="B15" t="s">
-        <v>393</v>
+        <v>359</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>397</v>
+        <v>363</v>
       </c>
       <c r="B16" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C16" t="s">
-        <v>398</v>
+        <v>364</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>399</v>
+        <v>365</v>
       </c>
       <c r="B17" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C17" t="s">
-        <v>400</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>401</v>
+        <v>367</v>
       </c>
       <c r="B18" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
       <c r="C18" t="s">
-        <v>402</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>403</v>
+        <v>369</v>
       </c>
       <c r="B19" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C19" t="s">
-        <v>404</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
       <c r="B20" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C20" t="s">
-        <v>406</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>407</v>
+        <v>373</v>
       </c>
       <c r="B21" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C21" t="s">
-        <v>408</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>409</v>
+        <v>375</v>
       </c>
       <c r="B22" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C22" t="s">
-        <v>410</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>411</v>
+        <v>377</v>
       </c>
       <c r="B23" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
       <c r="C23" t="s">
-        <v>412</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>413</v>
+        <v>379</v>
       </c>
       <c r="B24" t="s">
+        <v>346</v>
+      </c>
+      <c r="C24" t="s">
         <v>380</v>
-      </c>
-      <c r="C24" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>415</v>
+        <v>381</v>
       </c>
       <c r="B25" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="C25" t="s">
-        <v>416</v>
+        <v>382</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>417</v>
+        <v>383</v>
       </c>
       <c r="B26" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
       <c r="C26" t="s">
-        <v>418</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>419</v>
+        <v>385</v>
       </c>
       <c r="B27" t="s">
-        <v>393</v>
+        <v>359</v>
       </c>
       <c r="C27" t="s">
-        <v>420</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>